<commit_message>
AMA format of p values
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -2406,12 +2406,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ns (p = 0.054)</t>
+          <t>ns (p = .05)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>r = 0.19</t>
+          <t>r = .19</t>
         </is>
       </c>
     </row>
@@ -2433,12 +2433,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ns (p = 0.096)</t>
+          <t>ns (p = .10)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V = 0.19</t>
+          <t>V = .19</t>
         </is>
       </c>
     </row>
@@ -2460,12 +2460,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ns (p = 0.053)</t>
+          <t>ns (p = .05)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V = 0.23</t>
+          <t>V = .23</t>
         </is>
       </c>
     </row>
@@ -2489,12 +2489,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>p = 0.034</t>
+          <t>p = .03</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>r = 0.2</t>
+          <t>r = .2</t>
         </is>
       </c>
     </row>
@@ -2518,12 +2518,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ns (p = 0.087)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>r = 0.16</t>
+          <t>r = .16</t>
         </is>
       </c>
     </row>
@@ -2547,12 +2547,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ns (p = 0.051)</t>
+          <t>ns (p = .05)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>r = 0.19</t>
+          <t>r = .19</t>
         </is>
       </c>
     </row>
@@ -2661,12 +2661,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ns (p = 0.55)</t>
+          <t>ns (p = .55)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V = 0.13</t>
+          <t>V = .13</t>
         </is>
       </c>
     </row>
@@ -2702,12 +2702,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ns (p = 0.7)</t>
+          <t>ns (p = .70)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>η² = -0.018</t>
+          <t>η² = .018</t>
         </is>
       </c>
     </row>
@@ -2739,12 +2739,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ns (p = 0.98)</t>
+          <t>ns (p = .98)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>V = 0.025</t>
+          <t>V = .025</t>
         </is>
       </c>
     </row>
@@ -2776,12 +2776,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ns (p = 0.65)</t>
+          <t>ns (p = .65)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>V = 0.11</t>
+          <t>V = .11</t>
         </is>
       </c>
     </row>
@@ -2813,12 +2813,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ns (p = 0.68)</t>
+          <t>ns (p = .68)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>V = 0.1</t>
+          <t>V = .1</t>
         </is>
       </c>
     </row>
@@ -2850,12 +2850,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ns (p = 0.28)</t>
+          <t>ns (p = .28)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>V = 0.19</t>
+          <t>V = .19</t>
         </is>
       </c>
     </row>
@@ -2887,12 +2887,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ns (p = 0.18)</t>
+          <t>ns (p = .18)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>V = 0.21</t>
+          <t>V = .21</t>
         </is>
       </c>
     </row>
@@ -2924,12 +2924,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ns (p = 0.13)</t>
+          <t>ns (p = .13)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>V = 0.23</t>
+          <t>V = .23</t>
         </is>
       </c>
     </row>
@@ -2961,12 +2961,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ns (p = 0.55)</t>
+          <t>ns (p = .55)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>V = 0.13</t>
+          <t>V = .13</t>
         </is>
       </c>
     </row>
@@ -2998,12 +2998,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ns (p = 0.49)</t>
+          <t>ns (p = .49)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>V = 0.14</t>
+          <t>V = .14</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ns (p = 0.68)</t>
+          <t>ns (p = .68)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>V = 0.1</t>
+          <t>V = .1</t>
         </is>
       </c>
     </row>
@@ -3076,12 +3076,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ns (p = 0.54)</t>
+          <t>ns (p = .54)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>η² = -0.011</t>
+          <t>η² = .011</t>
         </is>
       </c>
     </row>
@@ -3113,12 +3113,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ns (p = 0.29)</t>
+          <t>ns (p = .29)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>V = 0.18</t>
+          <t>V = .18</t>
         </is>
       </c>
     </row>
@@ -3150,12 +3150,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ns (p = 0.21)</t>
+          <t>ns (p = .21)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>V = 0.2</t>
+          <t>V = .2</t>
         </is>
       </c>
     </row>
@@ -3187,12 +3187,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>V = 0.52</t>
+          <t>V = .52</t>
         </is>
       </c>
     </row>
@@ -3228,12 +3228,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>η² = 0.35</t>
+          <t>η² = .35</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>p = 0.0019</t>
+          <t>p = .002</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>V = 0.41</t>
+          <t>V = .41</t>
         </is>
       </c>
     </row>
@@ -3306,12 +3306,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ns (p = 0.11)</t>
+          <t>ns (p = .11)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>η² = 0.034</t>
+          <t>η² = .034</t>
         </is>
       </c>
     </row>
@@ -3347,12 +3347,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ns (p = 0.85)</t>
+          <t>ns (p = .85)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>η² = -0.024</t>
+          <t>η² = .024</t>
         </is>
       </c>
     </row>
@@ -3384,12 +3384,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>V = 0.61</t>
+          <t>V = .61</t>
         </is>
       </c>
     </row>
@@ -3498,12 +3498,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ns (p = 0.28)</t>
+          <t>ns (p = .28)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V = 0.19</t>
+          <t>V = .19</t>
         </is>
       </c>
     </row>
@@ -3539,12 +3539,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>p = 0.0029</t>
+          <t>p = .003</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>η² = 0.14</t>
+          <t>η² = .14</t>
         </is>
       </c>
     </row>
@@ -3580,12 +3580,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ns (p = 0.19)</t>
+          <t>ns (p = .19)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>η² = 0.018</t>
+          <t>η² = .018</t>
         </is>
       </c>
     </row>
@@ -3621,12 +3621,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ns (p = 0.82)</t>
+          <t>ns (p = .82)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>η² = -0.022</t>
+          <t>η² = .022</t>
         </is>
       </c>
     </row>
@@ -3662,12 +3662,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ns (p = 0.49)</t>
+          <t>ns (p = .49)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>η² = -0.008</t>
+          <t>η² = .008</t>
         </is>
       </c>
     </row>
@@ -3703,12 +3703,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ns (p = 0.28)</t>
+          <t>ns (p = .28)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>η² = 0.0078</t>
+          <t>η² = .0078</t>
         </is>
       </c>
     </row>
@@ -3744,12 +3744,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ns (p = 0.18)</t>
+          <t>ns (p = .18)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>η² = 0.021</t>
+          <t>η² = .021</t>
         </is>
       </c>
     </row>
@@ -3785,12 +3785,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ns (p = 0.13)</t>
+          <t>ns (p = .13)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>η² = 0.029</t>
+          <t>η² = .029</t>
         </is>
       </c>
     </row>
@@ -3826,12 +3826,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ns (p = 0.8)</t>
+          <t>ns (p = .80)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>η² = -0.022</t>
+          <t>η² = .022</t>
         </is>
       </c>
     </row>
@@ -3867,12 +3867,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ns (p = 0.11)</t>
+          <t>ns (p = .11)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>η² = 0.035</t>
+          <t>η² = .035</t>
         </is>
       </c>
     </row>
@@ -3951,12 +3951,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ns (p = 0.094)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V = 0.22</t>
+          <t>V = .22</t>
         </is>
       </c>
     </row>
@@ -3982,12 +3982,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>p = 0.034</t>
+          <t>p = .03</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V = 0.3</t>
+          <t>V = .3</t>
         </is>
       </c>
     </row>
@@ -4009,12 +4009,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ns (p = 0.066)</t>
+          <t>ns (p = .07)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V = 0.24</t>
+          <t>V = .24</t>
         </is>
       </c>
     </row>
@@ -4038,12 +4038,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>p = 0.0016</t>
+          <t>p = .002</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>r = 0.37</t>
+          <t>r = .37</t>
         </is>
       </c>
     </row>
@@ -4069,12 +4069,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>p = 0.013</t>
+          <t>p = .01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V = 0.34</t>
+          <t>V = .34</t>
         </is>
       </c>
     </row>
@@ -4096,12 +4096,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>p = 0.036</t>
+          <t>p = .04</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V = 0.27</t>
+          <t>V = .27</t>
         </is>
       </c>
     </row>
@@ -4125,12 +4125,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>p = 0.019</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>r = 0.27</t>
+          <t>r = .27</t>
         </is>
       </c>
     </row>
@@ -4152,12 +4152,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ns (p = 0.089)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V = 0.23</t>
+          <t>V = .23</t>
         </is>
       </c>
     </row>
@@ -4179,12 +4179,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V = 0.51</t>
+          <t>V = .51</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>r = 0.49</t>
+          <t>r = .49</t>
         </is>
       </c>
     </row>
@@ -4237,12 +4237,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>r = 0.51</t>
+          <t>r = .51</t>
         </is>
       </c>
     </row>
@@ -4266,12 +4266,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>p = 0.024</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>r = 0.26</t>
+          <t>r = .26</t>
         </is>
       </c>
     </row>
@@ -4295,12 +4295,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ns (p = 0.26)</t>
+          <t>ns (p = .26)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>r = 0.13</t>
+          <t>r = .13</t>
         </is>
       </c>
     </row>
@@ -4324,12 +4324,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ns (p = 1)</t>
+          <t>ns (p &gt; .99)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>r = 0.0013</t>
+          <t>r = .0013</t>
         </is>
       </c>
     </row>
@@ -4353,12 +4353,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ns (p = 0.26)</t>
+          <t>ns (p = .26)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>r = 0.13</t>
+          <t>r = .13</t>
         </is>
       </c>
     </row>
@@ -4382,12 +4382,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ns (p = 0.68)</t>
+          <t>ns (p = .68)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>r = 0.049</t>
+          <t>r = .049</t>
         </is>
       </c>
     </row>
@@ -4411,12 +4411,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ns (p = 0.47)</t>
+          <t>ns (p = .47)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>r = 0.085</t>
+          <t>r = .085</t>
         </is>
       </c>
     </row>
@@ -4440,12 +4440,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ns (p = 0.26)</t>
+          <t>ns (p = .26)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>r = 0.13</t>
+          <t>r = .13</t>
         </is>
       </c>
     </row>
@@ -4469,12 +4469,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ns (p = 0.77)</t>
+          <t>ns (p = .77)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>r = 0.035</t>
+          <t>r = .035</t>
         </is>
       </c>
     </row>
@@ -4498,12 +4498,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ns (p = 0.72)</t>
+          <t>ns (p = .72)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>r = 0.042</t>
+          <t>r = .042</t>
         </is>
       </c>
     </row>
@@ -4527,12 +4527,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ns (p = 0.66)</t>
+          <t>ns (p = .66)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>r = 0.053</t>
+          <t>r = .053</t>
         </is>
       </c>
     </row>
@@ -4556,12 +4556,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ns (p = 0.19)</t>
+          <t>ns (p = .19)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>r = 0.15</t>
+          <t>r = .15</t>
         </is>
       </c>
     </row>
@@ -4585,12 +4585,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ns (p = 0.78)</t>
+          <t>ns (p = .78)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>r = 0.034</t>
+          <t>r = .034</t>
         </is>
       </c>
     </row>
@@ -4669,12 +4669,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>p = 0.011</t>
+          <t>p = .01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V = 0.33</t>
+          <t>V = .33</t>
         </is>
       </c>
     </row>
@@ -4698,12 +4698,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>p = 0.0016</t>
+          <t>p = .002</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>r = 0.37</t>
+          <t>r = .37</t>
         </is>
       </c>
     </row>
@@ -4725,12 +4725,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>p = 0.0013</t>
+          <t>p = .001</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V = 0.42</t>
+          <t>V = .42</t>
         </is>
       </c>
     </row>
@@ -4754,12 +4754,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>p = 0.022</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>r = 0.27</t>
+          <t>r = .27</t>
         </is>
       </c>
     </row>
@@ -4781,12 +4781,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ns (p = 0.077)</t>
+          <t>ns (p = .08)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V = 0.24</t>
+          <t>V = .24</t>
         </is>
       </c>
     </row>
@@ -4808,12 +4808,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>p = 0.034</t>
+          <t>p = .03</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V = 0.28</t>
+          <t>V = .28</t>
         </is>
       </c>
     </row>
@@ -4837,12 +4837,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>p = 0.0051</t>
+          <t>p = .005</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>r = 0.33</t>
+          <t>r = .33</t>
         </is>
       </c>
     </row>
@@ -4866,12 +4866,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>p = 0.027</t>
+          <t>p = .03</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>r = 0.26</t>
+          <t>r = .26</t>
         </is>
       </c>
     </row>
@@ -4895,12 +4895,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>p = 0.031</t>
+          <t>p = .03</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>r = 0.25</t>
+          <t>r = .25</t>
         </is>
       </c>
     </row>
@@ -4924,12 +4924,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>p = 0.0064</t>
+          <t>p = .006</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>r = 0.32</t>
+          <t>r = .32</t>
         </is>
       </c>
     </row>
@@ -4953,12 +4953,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ns (p = 0.054)</t>
+          <t>ns (p = .05)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>r = 0.23</t>
+          <t>r = .23</t>
         </is>
       </c>
     </row>
@@ -5052,12 +5052,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ns (p = 0.087)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>V = 0.26</t>
+          <t>V = .26</t>
         </is>
       </c>
     </row>
@@ -5084,12 +5084,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ns (p = 0.087)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>V = 0.26</t>
+          <t>V = .26</t>
         </is>
       </c>
     </row>
@@ -5116,12 +5116,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ns (p = 0.091)</t>
+          <t>ns (p = .09)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>V = 0.25</t>
+          <t>V = .25</t>
         </is>
       </c>
     </row>
@@ -5151,12 +5151,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>p = 0.048</t>
+          <t>p = .048</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>η² = 0.058</t>
+          <t>η² = .058</t>
         </is>
       </c>
     </row>
@@ -5183,12 +5183,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>p = 0.017</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V = 0.33</t>
+          <t>V = .33</t>
         </is>
       </c>
     </row>
@@ -5218,12 +5218,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>η² = 0.31</t>
+          <t>η² = .31</t>
         </is>
       </c>
     </row>
@@ -5250,12 +5250,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>V = 0.51</t>
+          <t>V = .51</t>
         </is>
       </c>
     </row>
@@ -5282,12 +5282,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>p = 0.0055</t>
+          <t>p = .006</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>V = 0.37</t>
+          <t>V = .37</t>
         </is>
       </c>
     </row>
@@ -5314,12 +5314,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>p = 0.0083</t>
+          <t>p = .008</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>V = 0.36</t>
+          <t>V = .36</t>
         </is>
       </c>
     </row>
@@ -5346,12 +5346,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>p = 0.024</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>V = 0.32</t>
+          <t>V = .32</t>
         </is>
       </c>
     </row>
@@ -5378,12 +5378,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>V = 0.57</t>
+          <t>V = .57</t>
         </is>
       </c>
     </row>
@@ -5413,12 +5413,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>η² = 0.34</t>
+          <t>η² = .34</t>
         </is>
       </c>
     </row>
@@ -5445,12 +5445,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p &lt; .001</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>V = 0.57</t>
+          <t>V = .57</t>
         </is>
       </c>
     </row>
@@ -5477,12 +5477,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ns (p = 0.099)</t>
+          <t>ns (p = .10)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>V = 0.25</t>
+          <t>V = .25</t>
         </is>
       </c>
     </row>
@@ -5512,12 +5512,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>p = 0.015</t>
+          <t>p = .02</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>η² = 0.09</t>
+          <t>η² = .09</t>
         </is>
       </c>
     </row>
@@ -5544,12 +5544,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>p = 0.012</t>
+          <t>p = .01</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>V = 0.35</t>
+          <t>V = .35</t>
         </is>
       </c>
     </row>

</xml_diff>